<commit_message>
Upload two ways to get fan-in fan-out
One is create a ClassCallGraph based on CallGraph.
Another is based on ASM.
</commit_message>
<xml_diff>
--- a/submission/code-clone-detection/FileComparision.xlsx
+++ b/submission/code-clone-detection/FileComparision.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/home/IdeaProjects/COM6523/individual-project/submission/code-clone-detection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96961671-D7D5-C44E-89DE-E2920045E5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1118CB-F80D-B54E-A09D-FA712DEA5D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16000"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FileComparision" sheetId="1" r:id="rId1"/>
@@ -448,7 +448,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -973,27 +973,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1001,16 +981,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1353,17 +1323,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.6640625" customWidth="1"/>
-    <col min="2" max="2" width="80.5" customWidth="1"/>
+    <col min="1" max="1" width="41.5" customWidth="1"/>
+    <col min="2" max="2" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -5155,18 +5125,18 @@
     <sortCondition descending="1" ref="C2:C344"/>
   </sortState>
   <conditionalFormatting sqref="C2">
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="chrono/">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="chrono/">
       <formula>NOT(ISERROR(SEARCH("chrono/",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C344">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="chrono/">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="chrono/">
       <formula>NOT(ISERROR(SEARCH("chrono/",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="base/">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="base/">
       <formula>NOT(ISERROR(SEARCH("base/",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="field/">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="field/">
       <formula>NOT(ISERROR(SEARCH("field/",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>